<commit_message>
Add multi-index and multi-table functions into gen datasets script
</commit_message>
<xml_diff>
--- a/long_first/synthetic_dataset_1.xlsx
+++ b/long_first/synthetic_dataset_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -28,6 +28,12 @@
     <t>Value</t>
   </si>
   <si>
+    <t>not a date</t>
+  </si>
+  <si>
+    <t>yesterday</t>
+  </si>
+  <si>
     <t>TV</t>
   </si>
   <si>
@@ -40,13 +46,13 @@
     <t>GRPs</t>
   </si>
   <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>ten</t>
+  </si>
+  <si>
     <t>one hundred</t>
-  </si>
-  <si>
-    <t>NaN</t>
-  </si>
-  <si>
-    <t>ten</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,430 +436,688 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>46123</v>
+        <v>46022</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>107</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:4">
+      <c r="A3" s="2">
+        <v>46015</v>
+      </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>66</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>46088</v>
+        <v>46008</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>46109</v>
+        <v>46043</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>46095</v>
+        <v>46022</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2">
-        <v>46095</v>
-      </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D7">
-        <v>188</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>46116</v>
+        <v>46001</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D8">
-        <v>190</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>46109</v>
+        <v>46036</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>46130</v>
+        <v>45966</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>46137</v>
+        <v>45980</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>46130</v>
+        <v>45994</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
       </c>
       <c r="D12">
-        <v>189</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>46102</v>
+        <v>46015</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>46102</v>
+        <v>45994</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>125</v>
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4">
+      <c r="A15" s="2">
+        <v>45973</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>46088</v>
+        <v>46015</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D16">
-        <v>196</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>46116</v>
+        <v>46008</v>
       </c>
       <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2">
-        <v>46088</v>
-      </c>
       <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>46116</v>
+        <v>46001</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>46116</v>
+        <v>45973</v>
       </c>
       <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21">
         <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="2">
-        <v>46102</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>46095</v>
+        <v>46036</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D22">
-        <v>92</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>46088</v>
+        <v>45994</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>46095</v>
+        <v>45987</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>46109</v>
+        <v>46001</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:4">
+      <c r="A26" s="2">
+        <v>46036</v>
+      </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>46123</v>
+        <v>45980</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="2">
-        <v>46102</v>
+      <c r="A28" t="s">
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4">
+      <c r="A29" s="2">
+        <v>45980</v>
+      </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D29">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>46137</v>
+        <v>46043</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>46137</v>
+        <v>45973</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
       </c>
       <c r="D31">
-        <v>188</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:4">
+      <c r="A32" s="2">
+        <v>46015</v>
+      </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>46137</v>
+        <v>46008</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>46109</v>
+        <v>46001</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>46130</v>
+        <v>45973</v>
       </c>
       <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2">
+        <v>46043</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2">
+        <v>45966</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2">
+        <v>46022</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="2">
+        <v>46043</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2">
+        <v>46022</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2">
+        <v>46008</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2">
+        <v>45994</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2">
+        <v>46015</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2">
+        <v>46008</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2">
+        <v>46036</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48">
         <v>5</v>
       </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" t="s">
-        <v>8</v>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2">
+        <v>45987</v>
+      </c>
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2">
+        <v>46008</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>